<commit_message>
continue to adapt code to v17
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v17.xlsx
+++ b/Template_CoMoCOVID-19App_v17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4586DC0E-938C-5646-A662-051D69EEED90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1390D-B536-FB4C-9807-1C83F1F0C3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="640" windowWidth="18700" windowHeight="17500" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="10420" yWindow="640" windowWidth="24880" windowHeight="20680" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3802,9 +3802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -4120,7 +4118,7 @@
   </sheetPr>
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -8655,7 +8653,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
improved static interventions plot
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v17.xlsx
+++ b/Template_CoMoCOVID-19App_v17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1390D-B536-FB4C-9807-1C83F1F0C3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF0776F-07E2-5049-95A5-4AAB3995960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10420" yWindow="640" windowWidth="24880" windowHeight="20680" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="482">
   <si>
     <t>5-10 y.o.</t>
   </si>
@@ -2949,17 +2949,70 @@
   </si>
   <si>
     <t>0-5 y.o.</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>sample_size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parameters sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Added sample_size.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(v17)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sample Size</t>
+    </r>
+  </si>
+  <si>
+    <t>(a)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3050,6 +3103,18 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -3090,12 +3155,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3103,6 +3162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3200,7 +3265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3338,19 +3403,13 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3386,16 +3445,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3416,12 +3472,32 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3466,16 +3542,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3490,14 +3556,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="E1:F15" xr:uid="{2E89BE7F-E667-6946-928D-DC5AB4119A65}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3800,9 +3866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -3813,6 +3881,9 @@
       <c r="A1" s="5" t="s">
         <v>438</v>
       </c>
+      <c r="B1" s="95" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="21">
       <c r="A2" s="3" t="s">
@@ -3868,73 +3939,73 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="94" t="s">
         <v>443</v>
       </c>
       <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="94" t="s">
         <v>444</v>
       </c>
       <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="94" t="s">
         <v>445</v>
       </c>
       <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="94" t="s">
         <v>446</v>
       </c>
       <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="94" t="s">
         <v>447</v>
       </c>
       <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="94" t="s">
         <v>448</v>
       </c>
       <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="94" t="s">
         <v>449</v>
       </c>
       <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="94" t="s">
         <v>450</v>
       </c>
       <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="94" t="s">
         <v>451</v>
       </c>
       <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="94" t="s">
         <v>452</v>
       </c>
       <c r="F24" s="40"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="94" t="s">
         <v>453</v>
       </c>
       <c r="F25" s="40"/>
     </row>
     <row r="26" spans="1:6" s="39" customFormat="1">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="94" t="s">
         <v>454</v>
       </c>
       <c r="B26"/>
@@ -3942,167 +4013,172 @@
       <c r="F26" s="40"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="94" t="s">
         <v>455</v>
       </c>
       <c r="F27" s="40"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="94" t="s">
         <v>456</v>
       </c>
       <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="87" t="s">
+      <c r="A29" s="94" t="s">
         <v>457</v>
       </c>
       <c r="F29" s="40"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="94" t="s">
         <v>458</v>
       </c>
       <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="87" t="s">
+      <c r="A31" s="94" t="s">
         <v>459</v>
       </c>
       <c r="F31" s="40"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="94" t="s">
         <v>460</v>
       </c>
       <c r="F32" s="40"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="94" t="s">
         <v>461</v>
       </c>
       <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="94" t="s">
         <v>462</v>
       </c>
       <c r="F34" s="40"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="94" t="s">
         <v>463</v>
       </c>
       <c r="F35" s="40"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="80" t="s">
+      <c r="A37" s="78" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34">
-      <c r="A38" s="89" t="s">
+      <c r="A38" s="86" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="34">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="87" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="87" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="80"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="83" t="s">
+    <row r="41" spans="1:6" ht="17">
+      <c r="A41" s="87" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="78"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="81" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="34">
-      <c r="A44" s="38" t="s">
+    <row r="45" spans="1:6" ht="34">
+      <c r="A45" s="38" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="17">
-      <c r="A45" s="38" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17">
       <c r="A46" s="38" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17">
       <c r="A47" s="38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17">
+      <c r="A48" s="38" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="34">
-      <c r="A48" s="38" t="s">
+    <row r="49" spans="1:1" ht="34">
+      <c r="A49" s="38" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="78" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" s="76" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="40" t="s">
+    <row r="52" spans="1:1">
+      <c r="A52" s="40" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="79" t="s">
+    <row r="54" spans="1:1">
+      <c r="A54" s="77" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="34">
-      <c r="A55" s="38" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="34">
       <c r="A56" s="38" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="34">
+      <c r="A57" s="38" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="68">
-      <c r="A57" s="38" t="s">
+    <row r="58" spans="1:1" ht="68">
+      <c r="A58" s="38" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="38"/>
-    </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="79" t="s">
+      <c r="A59" s="38"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="77" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4174,7 +4250,7 @@
         <f>IF(A2="","",VLOOKUP(A2,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>contacts</v>
       </c>
-      <c r="F2" s="85"/>
+      <c r="F2" s="83"/>
       <c r="G2" s="1" t="s">
         <v>277</v>
       </c>
@@ -4196,7 +4272,7 @@
         <f>IF(A3="","",VLOOKUP(A3,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F3" s="86"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="1" t="s">
         <v>277</v>
       </c>
@@ -4218,7 +4294,7 @@
         <f>IF(A4="","",VLOOKUP(A4,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>contacts</v>
       </c>
-      <c r="F4" s="86"/>
+      <c r="F4" s="84"/>
       <c r="G4" s="1" t="s">
         <v>277</v>
       </c>
@@ -4240,7 +4316,7 @@
         <f>IF(A5="","",VLOOKUP(A5,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F5" s="86"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="1" t="s">
         <v>277</v>
       </c>
@@ -4262,7 +4338,7 @@
         <f>IF(A6="","",VLOOKUP(A6,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F6" s="86"/>
+      <c r="F6" s="84"/>
       <c r="G6" s="1" t="s">
         <v>278</v>
       </c>
@@ -4284,7 +4360,7 @@
         <f>IF(A7="","",VLOOKUP(A7,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F7" s="86"/>
+      <c r="F7" s="84"/>
       <c r="G7" s="1" t="s">
         <v>278</v>
       </c>
@@ -4306,7 +4382,7 @@
         <f>IF(A8="","",VLOOKUP(A8,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F8" s="86"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="1" t="s">
         <v>278</v>
       </c>
@@ -4328,7 +4404,7 @@
         <f>IF(A9="","",VLOOKUP(A9,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>contacts</v>
       </c>
-      <c r="F9" s="86"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="1" t="s">
         <v>278</v>
       </c>
@@ -4350,7 +4426,7 @@
         <f>IF(A10="","",VLOOKUP(A10,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F10" s="86"/>
+      <c r="F10" s="84"/>
       <c r="G10" s="1" t="s">
         <v>278</v>
       </c>
@@ -4372,7 +4448,7 @@
         <f>IF(A11="","",VLOOKUP(A11,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F11" s="86"/>
+      <c r="F11" s="84"/>
       <c r="G11" s="1" t="s">
         <v>278</v>
       </c>
@@ -4394,7 +4470,7 @@
         <f>IF(A12="","",VLOOKUP(A12,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F12" s="86"/>
+      <c r="F12" s="84"/>
       <c r="G12" s="1" t="s">
         <v>278</v>
       </c>
@@ -4416,7 +4492,7 @@
         <f>IF(A13="","",VLOOKUP(A13,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>thousand tests</v>
       </c>
-      <c r="F13" s="86" t="s">
+      <c r="F13" s="84" t="s">
         <v>468</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -4440,7 +4516,7 @@
         <f>IF(A14="","",VLOOKUP(A14,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F14" s="86" t="s">
+      <c r="F14" s="84" t="s">
         <v>441</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -4464,7 +4540,7 @@
         <f>IF(A15="","",VLOOKUP(A15,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F15" s="86"/>
+      <c r="F15" s="84"/>
       <c r="G15" s="1" t="s">
         <v>278</v>
       </c>
@@ -4486,7 +4562,7 @@
         <f>IF(A16="","",VLOOKUP(A16,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v>%</v>
       </c>
-      <c r="F16" s="86" t="s">
+      <c r="F16" s="84" t="s">
         <v>440</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -4502,7 +4578,7 @@
         <f>IF(A17="","",VLOOKUP(A17,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
@@ -4514,7 +4590,7 @@
         <f>IF(A18="","",VLOOKUP(A18,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F18" s="85"/>
+      <c r="F18" s="83"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
@@ -4526,7 +4602,7 @@
         <f>IF(A19="","",VLOOKUP(A19,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F19" s="85"/>
+      <c r="F19" s="83"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
@@ -4538,7 +4614,7 @@
         <f>IF(A20="","",VLOOKUP(A20,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F20" s="85"/>
+      <c r="F20" s="83"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
@@ -4550,7 +4626,7 @@
         <f>IF(A21="","",VLOOKUP(A21,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F21" s="85"/>
+      <c r="F21" s="83"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
@@ -4562,7 +4638,7 @@
         <f>IF(A22="","",VLOOKUP(A22,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F22" s="85"/>
+      <c r="F22" s="83"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
@@ -4574,7 +4650,7 @@
         <f>IF(A23="","",VLOOKUP(A23,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F23" s="85"/>
+      <c r="F23" s="83"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
@@ -4586,7 +4662,7 @@
         <f>IF(A24="","",VLOOKUP(A24,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F24" s="85"/>
+      <c r="F24" s="83"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
@@ -4598,7 +4674,7 @@
         <f>IF(A25="","",VLOOKUP(A25,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F25" s="85"/>
+      <c r="F25" s="83"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
@@ -4610,7 +4686,7 @@
         <f>IF(A26="","",VLOOKUP(A26,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F26" s="85"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
@@ -4622,7 +4698,7 @@
         <f>IF(A27="","",VLOOKUP(A27,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F27" s="85"/>
+      <c r="F27" s="83"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7">
@@ -4634,7 +4710,7 @@
         <f>IF(A28="","",VLOOKUP(A28,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F28" s="85"/>
+      <c r="F28" s="83"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7">
@@ -4646,7 +4722,7 @@
         <f>IF(A29="","",VLOOKUP(A29,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F29" s="85"/>
+      <c r="F29" s="83"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
@@ -4658,7 +4734,7 @@
         <f>IF(A30="","",VLOOKUP(A30,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F30" s="85"/>
+      <c r="F30" s="83"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7">
@@ -4670,7 +4746,7 @@
         <f>IF(A31="","",VLOOKUP(A31,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F31" s="85"/>
+      <c r="F31" s="83"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7">
@@ -4682,7 +4758,7 @@
         <f>IF(A32="","",VLOOKUP(A32,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F32" s="85"/>
+      <c r="F32" s="83"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7">
@@ -4694,7 +4770,7 @@
         <f>IF(A33="","",VLOOKUP(A33,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F33" s="85"/>
+      <c r="F33" s="83"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7">
@@ -4706,7 +4782,7 @@
         <f>IF(A34="","",VLOOKUP(A34,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F34" s="85"/>
+      <c r="F34" s="83"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
@@ -4718,7 +4794,7 @@
         <f>IF(A35="","",VLOOKUP(A35,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F35" s="85"/>
+      <c r="F35" s="83"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7">
@@ -4730,7 +4806,7 @@
         <f>IF(A36="","",VLOOKUP(A36,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F36" s="85"/>
+      <c r="F36" s="83"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7">
@@ -4742,7 +4818,7 @@
         <f>IF(A37="","",VLOOKUP(A37,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F37" s="85"/>
+      <c r="F37" s="83"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7">
@@ -4754,7 +4830,7 @@
         <f>IF(A38="","",VLOOKUP(A38,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F38" s="85"/>
+      <c r="F38" s="83"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7">
@@ -4766,7 +4842,7 @@
         <f>IF(A39="","",VLOOKUP(A39,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F39" s="85"/>
+      <c r="F39" s="83"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7">
@@ -4778,7 +4854,7 @@
         <f>IF(A40="","",VLOOKUP(A40,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F40" s="85"/>
+      <c r="F40" s="83"/>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7">
@@ -4790,7 +4866,7 @@
         <f>IF(A41="","",VLOOKUP(A41,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F41" s="85"/>
+      <c r="F41" s="83"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7">
@@ -4802,7 +4878,7 @@
         <f>IF(A42="","",VLOOKUP(A42,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F42" s="85"/>
+      <c r="F42" s="83"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7">
@@ -4814,7 +4890,7 @@
         <f>IF(A43="","",VLOOKUP(A43,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F43" s="85"/>
+      <c r="F43" s="83"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7">
@@ -4826,7 +4902,7 @@
         <f>IF(A44="","",VLOOKUP(A44,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F44" s="85"/>
+      <c r="F44" s="83"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7">
@@ -4838,7 +4914,7 @@
         <f>IF(A45="","",VLOOKUP(A45,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F45" s="85"/>
+      <c r="F45" s="83"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7">
@@ -4850,7 +4926,7 @@
         <f>IF(A46="","",VLOOKUP(A46,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F46" s="85"/>
+      <c r="F46" s="83"/>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7">
@@ -4862,7 +4938,7 @@
         <f>IF(A47="","",VLOOKUP(A47,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F47" s="85"/>
+      <c r="F47" s="83"/>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7">
@@ -4874,7 +4950,7 @@
         <f>IF(A48="","",VLOOKUP(A48,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F48" s="85"/>
+      <c r="F48" s="83"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7">
@@ -4886,7 +4962,7 @@
         <f>IF(A49="","",VLOOKUP(A49,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F49" s="85"/>
+      <c r="F49" s="83"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7">
@@ -4898,7 +4974,7 @@
         <f>IF(A50="","",VLOOKUP(A50,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F50" s="85"/>
+      <c r="F50" s="83"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7">
@@ -4910,7 +4986,7 @@
         <f>IF(A51="","",VLOOKUP(A51,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F51" s="85"/>
+      <c r="F51" s="83"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7">
@@ -4922,7 +4998,7 @@
         <f>IF(A52="","",VLOOKUP(A52,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F52" s="85"/>
+      <c r="F52" s="83"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7">
@@ -4934,7 +5010,7 @@
         <f>IF(A53="","",VLOOKUP(A53,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F53" s="85"/>
+      <c r="F53" s="83"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7">
@@ -4946,7 +5022,7 @@
         <f>IF(A54="","",VLOOKUP(A54,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F54" s="85"/>
+      <c r="F54" s="83"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7">
@@ -4958,7 +5034,7 @@
         <f>IF(A55="","",VLOOKUP(A55,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F55" s="85"/>
+      <c r="F55" s="83"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7">
@@ -4970,7 +5046,7 @@
         <f>IF(A56="","",VLOOKUP(A56,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F56" s="85"/>
+      <c r="F56" s="83"/>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7">
@@ -4982,7 +5058,7 @@
         <f>IF(A57="","",VLOOKUP(A57,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F57" s="85"/>
+      <c r="F57" s="83"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7">
@@ -4994,7 +5070,7 @@
         <f>IF(A58="","",VLOOKUP(A58,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F58" s="85"/>
+      <c r="F58" s="83"/>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7">
@@ -5006,7 +5082,7 @@
         <f>IF(A59="","",VLOOKUP(A59,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F59" s="85"/>
+      <c r="F59" s="83"/>
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7">
@@ -5018,7 +5094,7 @@
         <f>IF(A60="","",VLOOKUP(A60,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F60" s="85"/>
+      <c r="F60" s="83"/>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7">
@@ -5030,7 +5106,7 @@
         <f>IF(A61="","",VLOOKUP(A61,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F61" s="85"/>
+      <c r="F61" s="83"/>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7">
@@ -5042,7 +5118,7 @@
         <f>IF(A62="","",VLOOKUP(A62,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F62" s="85"/>
+      <c r="F62" s="83"/>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7">
@@ -5054,7 +5130,7 @@
         <f>IF(A63="","",VLOOKUP(A63,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F63" s="85"/>
+      <c r="F63" s="83"/>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7">
@@ -5066,7 +5142,7 @@
         <f>IF(A64="","",VLOOKUP(A64,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F64" s="85"/>
+      <c r="F64" s="83"/>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7">
@@ -5078,7 +5154,7 @@
         <f>IF(A65="","",VLOOKUP(A65,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F65" s="85"/>
+      <c r="F65" s="83"/>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7">
@@ -5090,7 +5166,7 @@
         <f>IF(A66="","",VLOOKUP(A66,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F66" s="85"/>
+      <c r="F66" s="83"/>
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7">
@@ -5102,7 +5178,7 @@
         <f>IF(A67="","",VLOOKUP(A67,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F67" s="85"/>
+      <c r="F67" s="83"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7">
@@ -5114,7 +5190,7 @@
         <f>IF(A68="","",VLOOKUP(A68,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F68" s="85"/>
+      <c r="F68" s="83"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7">
@@ -5126,7 +5202,7 @@
         <f>IF(A69="","",VLOOKUP(A69,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F69" s="85"/>
+      <c r="F69" s="83"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7">
@@ -5138,7 +5214,7 @@
         <f>IF(A70="","",VLOOKUP(A70,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F70" s="85"/>
+      <c r="F70" s="83"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7">
@@ -5150,7 +5226,7 @@
         <f>IF(A71="","",VLOOKUP(A71,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F71" s="85"/>
+      <c r="F71" s="83"/>
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7">
@@ -5162,7 +5238,7 @@
         <f>IF(A72="","",VLOOKUP(A72,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F72" s="85"/>
+      <c r="F72" s="83"/>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7">
@@ -5174,7 +5250,7 @@
         <f>IF(A73="","",VLOOKUP(A73,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F73" s="85"/>
+      <c r="F73" s="83"/>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7">
@@ -5186,7 +5262,7 @@
         <f>IF(A74="","",VLOOKUP(A74,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F74" s="85"/>
+      <c r="F74" s="83"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7">
@@ -5198,7 +5274,7 @@
         <f>IF(A75="","",VLOOKUP(A75,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F75" s="85"/>
+      <c r="F75" s="83"/>
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7">
@@ -5210,7 +5286,7 @@
         <f>IF(A76="","",VLOOKUP(A76,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F76" s="85"/>
+      <c r="F76" s="83"/>
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="1:7">
@@ -5222,7 +5298,7 @@
         <f>IF(A77="","",VLOOKUP(A77,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F77" s="85"/>
+      <c r="F77" s="83"/>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7">
@@ -5234,7 +5310,7 @@
         <f>IF(A78="","",VLOOKUP(A78,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F78" s="85"/>
+      <c r="F78" s="83"/>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7">
@@ -5246,7 +5322,7 @@
         <f>IF(A79="","",VLOOKUP(A79,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F79" s="85"/>
+      <c r="F79" s="83"/>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7">
@@ -5258,7 +5334,7 @@
         <f>IF(A80="","",VLOOKUP(A80,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F80" s="85"/>
+      <c r="F80" s="83"/>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="1:7">
@@ -5270,7 +5346,7 @@
         <f>IF(A81="","",VLOOKUP(A81,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F81" s="85"/>
+      <c r="F81" s="83"/>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7">
@@ -5282,7 +5358,7 @@
         <f>IF(A82="","",VLOOKUP(A82,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F82" s="85"/>
+      <c r="F82" s="83"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7">
@@ -5294,7 +5370,7 @@
         <f>IF(A83="","",VLOOKUP(A83,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F83" s="85"/>
+      <c r="F83" s="83"/>
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="1:7">
@@ -5306,7 +5382,7 @@
         <f>IF(A84="","",VLOOKUP(A84,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F84" s="85"/>
+      <c r="F84" s="83"/>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7">
@@ -5318,7 +5394,7 @@
         <f>IF(A85="","",VLOOKUP(A85,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F85" s="85"/>
+      <c r="F85" s="83"/>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7">
@@ -5330,7 +5406,7 @@
         <f>IF(A86="","",VLOOKUP(A86,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F86" s="85"/>
+      <c r="F86" s="83"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="1:7">
@@ -5342,7 +5418,7 @@
         <f>IF(A87="","",VLOOKUP(A87,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F87" s="85"/>
+      <c r="F87" s="83"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7">
@@ -5354,7 +5430,7 @@
         <f>IF(A88="","",VLOOKUP(A88,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F88" s="85"/>
+      <c r="F88" s="83"/>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7">
@@ -5366,7 +5442,7 @@
         <f>IF(A89="","",VLOOKUP(A89,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F89" s="85"/>
+      <c r="F89" s="83"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7">
@@ -5378,7 +5454,7 @@
         <f>IF(A90="","",VLOOKUP(A90,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F90" s="85"/>
+      <c r="F90" s="83"/>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7">
@@ -5390,7 +5466,7 @@
         <f>IF(A91="","",VLOOKUP(A91,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F91" s="85"/>
+      <c r="F91" s="83"/>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7">
@@ -5402,7 +5478,7 @@
         <f>IF(A92="","",VLOOKUP(A92,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F92" s="85"/>
+      <c r="F92" s="83"/>
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="1:7">
@@ -5414,7 +5490,7 @@
         <f>IF(A93="","",VLOOKUP(A93,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F93" s="85"/>
+      <c r="F93" s="83"/>
       <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7">
@@ -5426,7 +5502,7 @@
         <f>IF(A94="","",VLOOKUP(A94,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F94" s="85"/>
+      <c r="F94" s="83"/>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7">
@@ -5438,7 +5514,7 @@
         <f>IF(A95="","",VLOOKUP(A95,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F95" s="85"/>
+      <c r="F95" s="83"/>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7">
@@ -5450,7 +5526,7 @@
         <f>IF(A96="","",VLOOKUP(A96,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F96" s="85"/>
+      <c r="F96" s="83"/>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7">
@@ -5462,7 +5538,7 @@
         <f>IF(A97="","",VLOOKUP(A97,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F97" s="85"/>
+      <c r="F97" s="83"/>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7">
@@ -5474,7 +5550,7 @@
         <f>IF(A98="","",VLOOKUP(A98,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F98" s="85"/>
+      <c r="F98" s="83"/>
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7">
@@ -5486,7 +5562,7 @@
         <f>IF(A99="","",VLOOKUP(A99,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F99" s="85"/>
+      <c r="F99" s="83"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="1:7">
@@ -5498,12 +5574,12 @@
         <f>IF(A100="","",VLOOKUP(A100,HIDDEN!$E$2:$F$15,2,FALSE))</f>
         <v/>
       </c>
-      <c r="F100" s="85"/>
+      <c r="F100" s="83"/>
       <c r="G100" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F100">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(OR($A2 = "Vaccination", $A2 = "School Closures",  $A2 = "Mass Testing"))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5558,10 +5634,10 @@
       <c r="C1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="82" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="82" t="s">
         <v>338</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -7586,13 +7662,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="170">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="72" t="s">
         <v>101</v>
       </c>
     </row>
@@ -7600,10 +7676,10 @@
       <c r="A2" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="B2" s="80">
+      <c r="B2" s="78">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="C2" s="80">
+      <c r="C2" s="78">
         <v>0</v>
       </c>
     </row>
@@ -7611,10 +7687,10 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="80">
+      <c r="B3" s="78">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="78">
         <v>0</v>
       </c>
     </row>
@@ -7622,10 +7698,10 @@
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="80">
+      <c r="B4" s="78">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C4" s="80">
+      <c r="C4" s="78">
         <v>0.04</v>
       </c>
     </row>
@@ -7633,10 +7709,10 @@
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="78">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="78">
         <v>0.04</v>
       </c>
     </row>
@@ -7644,10 +7720,10 @@
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="80">
+      <c r="B6" s="78">
         <v>3.1E-2</v>
       </c>
-      <c r="C6" s="80">
+      <c r="C6" s="78">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -7655,10 +7731,10 @@
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="80">
+      <c r="B7" s="78">
         <v>3.1E-2</v>
       </c>
-      <c r="C7" s="80">
+      <c r="C7" s="78">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -7666,10 +7742,10 @@
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="80">
+      <c r="B8" s="78">
         <v>0.26</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="78">
         <v>3.43</v>
       </c>
     </row>
@@ -7677,10 +7753,10 @@
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="80">
+      <c r="B9" s="78">
         <v>0.26</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="78">
         <v>3.43</v>
       </c>
     </row>
@@ -7688,10 +7764,10 @@
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="80">
+      <c r="B10" s="78">
         <v>0.48</v>
       </c>
-      <c r="C10" s="80">
+      <c r="C10" s="78">
         <v>4.25</v>
       </c>
     </row>
@@ -7699,10 +7775,10 @@
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="80">
+      <c r="B11" s="78">
         <v>0.48</v>
       </c>
-      <c r="C11" s="80">
+      <c r="C11" s="78">
         <v>4.25</v>
       </c>
     </row>
@@ -7710,10 +7786,10 @@
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="80">
+      <c r="B12" s="78">
         <v>0.6</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="78">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -7721,10 +7797,10 @@
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="80">
+      <c r="B13" s="78">
         <v>0.6</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="78">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -7732,10 +7808,10 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="80">
+      <c r="B14" s="78">
         <v>1.9</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="78">
         <v>11.8</v>
       </c>
     </row>
@@ -7743,10 +7819,10 @@
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="80">
+      <c r="B15" s="78">
         <v>1.9</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="78">
         <v>11.8</v>
       </c>
     </row>
@@ -7754,10 +7830,10 @@
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="80">
+      <c r="B16" s="78">
         <v>4.3</v>
       </c>
-      <c r="C16" s="80">
+      <c r="C16" s="78">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -7765,10 +7841,10 @@
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="80">
+      <c r="B17" s="78">
         <v>4.3</v>
       </c>
-      <c r="C17" s="80">
+      <c r="C17" s="78">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -7776,10 +7852,10 @@
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="80">
+      <c r="B18" s="78">
         <v>7.8</v>
       </c>
-      <c r="C18" s="80">
+      <c r="C18" s="78">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -7787,10 +7863,10 @@
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="80">
+      <c r="B19" s="78">
         <v>7.8</v>
       </c>
-      <c r="C19" s="80">
+      <c r="C19" s="78">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -7798,10 +7874,10 @@
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="80">
+      <c r="B20" s="78">
         <v>7.8</v>
       </c>
-      <c r="C20" s="80">
+      <c r="C20" s="78">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -7809,10 +7885,10 @@
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="80">
+      <c r="B21" s="78">
         <v>7.8</v>
       </c>
-      <c r="C21" s="80">
+      <c r="C21" s="78">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -7820,10 +7896,10 @@
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="80">
+      <c r="B22" s="78">
         <v>7.8</v>
       </c>
-      <c r="C22" s="80">
+      <c r="C22" s="78">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -7877,13 +7953,13 @@
       <c r="A2" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="B2" s="81">
+      <c r="B2" s="79">
         <v>3924000</v>
       </c>
-      <c r="C2" s="82">
-        <v>0</v>
-      </c>
-      <c r="D2" s="82">
+      <c r="C2" s="80">
+        <v>0</v>
+      </c>
+      <c r="D2" s="80">
         <v>2.3722458400227202E-6</v>
       </c>
     </row>
@@ -7891,13 +7967,13 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="81">
+      <c r="B3" s="79">
         <v>4120000</v>
       </c>
-      <c r="C3" s="82">
-        <v>0</v>
-      </c>
-      <c r="D3" s="82">
+      <c r="C3" s="80">
+        <v>0</v>
+      </c>
+      <c r="D3" s="80">
         <v>1.32905378016121E-7</v>
       </c>
     </row>
@@ -7905,13 +7981,13 @@
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="81">
+      <c r="B4" s="79">
         <v>3956000</v>
       </c>
-      <c r="C4" s="82">
-        <v>0</v>
-      </c>
-      <c r="D4" s="82">
+      <c r="C4" s="80">
+        <v>0</v>
+      </c>
+      <c r="D4" s="80">
         <v>2.7683021103459102E-7</v>
       </c>
     </row>
@@ -7919,13 +7995,13 @@
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="79">
         <v>3686000</v>
       </c>
-      <c r="C5" s="82">
+      <c r="C5" s="80">
         <v>1.82721457849836E-5</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="80">
         <v>5.9421612308889897E-7</v>
       </c>
     </row>
@@ -7933,13 +8009,13 @@
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="79">
         <v>4075000</v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="80">
         <v>7.3367682442901998E-5</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="80">
         <v>9.4061131337053795E-7</v>
       </c>
     </row>
@@ -7947,13 +8023,13 @@
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="79">
         <v>4484000</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="80">
         <v>1.2968766886415199E-4</v>
       </c>
-      <c r="D7" s="82">
+      <c r="D7" s="80">
         <v>1.22116449024625E-6</v>
       </c>
     </row>
@@ -7961,13 +8037,13 @@
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="81">
+      <c r="B8" s="79">
         <v>4707000</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="80">
         <v>1.4518112523224401E-4</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="80">
         <v>1.74496544750293E-6</v>
       </c>
     </row>
@@ -7975,13 +8051,13 @@
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="81">
+      <c r="B9" s="79">
         <v>4588000</v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="80">
         <v>8.5692103973881797E-5</v>
       </c>
-      <c r="D9" s="82">
+      <c r="D9" s="80">
         <v>2.3869666845092401E-6</v>
       </c>
     </row>
@@ -7989,13 +8065,13 @@
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="81">
+      <c r="B10" s="79">
         <v>4308000</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="80">
         <v>1.9320024124609101E-5</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="80">
         <v>3.9402680780452703E-6</v>
       </c>
     </row>
@@ -8003,13 +8079,13 @@
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="81">
+      <c r="B11" s="79">
         <v>4296000</v>
       </c>
-      <c r="C11" s="82">
+      <c r="C11" s="80">
         <v>1.2746046495028399E-6</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="80">
         <v>5.9906418526633501E-6</v>
       </c>
     </row>
@@ -8017,13 +8093,13 @@
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="81">
+      <c r="B12" s="79">
         <v>4635000</v>
       </c>
-      <c r="C12" s="82">
-        <v>0</v>
-      </c>
-      <c r="D12" s="82">
+      <c r="C12" s="80">
+        <v>0</v>
+      </c>
+      <c r="D12" s="80">
         <v>8.5059441930317695E-6</v>
       </c>
     </row>
@@ -8031,13 +8107,13 @@
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="81">
+      <c r="B13" s="79">
         <v>4539000</v>
       </c>
-      <c r="C13" s="82">
-        <v>0</v>
-      </c>
-      <c r="D13" s="82">
+      <c r="C13" s="80">
+        <v>0</v>
+      </c>
+      <c r="D13" s="80">
         <v>1.26668575743058E-5</v>
       </c>
     </row>
@@ -8045,13 +8121,13 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="81">
+      <c r="B14" s="79">
         <v>3905000</v>
       </c>
-      <c r="C14" s="82">
-        <v>0</v>
-      </c>
-      <c r="D14" s="82">
+      <c r="C14" s="80">
+        <v>0</v>
+      </c>
+      <c r="D14" s="80">
         <v>2.0472533414662599E-5</v>
       </c>
     </row>
@@ -8059,13 +8135,13 @@
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="81">
+      <c r="B15" s="79">
         <v>3382000</v>
       </c>
-      <c r="C15" s="82">
-        <v>0</v>
-      </c>
-      <c r="D15" s="82">
+      <c r="C15" s="80">
+        <v>0</v>
+      </c>
+      <c r="D15" s="80">
         <v>3.4000512436294603E-5</v>
       </c>
     </row>
@@ -8073,13 +8149,13 @@
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="81">
+      <c r="B16" s="79">
         <v>3388000</v>
       </c>
-      <c r="C16" s="82">
-        <v>0</v>
-      </c>
-      <c r="D16" s="82">
+      <c r="C16" s="80">
+        <v>0</v>
+      </c>
+      <c r="D16" s="80">
         <v>4.9617484749088298E-5</v>
       </c>
     </row>
@@ -8087,13 +8163,13 @@
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="81">
+      <c r="B17" s="79">
         <v>2442000</v>
       </c>
-      <c r="C17" s="82">
-        <v>0</v>
-      </c>
-      <c r="D17" s="82">
+      <c r="C17" s="80">
+        <v>0</v>
+      </c>
+      <c r="D17" s="80">
         <v>8.7449779441565906E-5</v>
       </c>
     </row>
@@ -8101,13 +8177,13 @@
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="81">
+      <c r="B18" s="79">
         <v>1737000</v>
       </c>
-      <c r="C18" s="82">
-        <v>0</v>
-      </c>
-      <c r="D18" s="82">
+      <c r="C18" s="80">
+        <v>0</v>
+      </c>
+      <c r="D18" s="80">
         <v>1.6171761126065301E-4</v>
       </c>
     </row>
@@ -8115,13 +8191,13 @@
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="81">
+      <c r="B19" s="79">
         <v>1078000</v>
       </c>
-      <c r="C19" s="82">
-        <v>0</v>
-      </c>
-      <c r="D19" s="82">
+      <c r="C19" s="80">
+        <v>0</v>
+      </c>
+      <c r="D19" s="80">
         <v>2.9461103089733202E-4</v>
       </c>
     </row>
@@ -8129,13 +8205,13 @@
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="81">
+      <c r="B20" s="79">
         <v>491000</v>
       </c>
-      <c r="C20" s="82">
-        <v>0</v>
-      </c>
-      <c r="D20" s="82">
+      <c r="C20" s="80">
+        <v>0</v>
+      </c>
+      <c r="D20" s="80">
         <v>4.9738551978041395E-4</v>
       </c>
     </row>
@@ -8143,13 +8219,13 @@
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="81">
+      <c r="B21" s="79">
         <v>130000</v>
       </c>
-      <c r="C21" s="82">
-        <v>0</v>
-      </c>
-      <c r="D21" s="82">
+      <c r="C21" s="80">
+        <v>0</v>
+      </c>
+      <c r="D21" s="80">
         <v>8.9717264255251901E-4</v>
       </c>
     </row>
@@ -8157,13 +8233,13 @@
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="81">
+      <c r="B22" s="79">
         <v>16000</v>
       </c>
-      <c r="C22" s="82">
-        <v>0</v>
-      </c>
-      <c r="D22" s="82">
+      <c r="C22" s="80">
+        <v>0</v>
+      </c>
+      <c r="D22" s="80">
         <v>7.2895277207392197E-3</v>
       </c>
     </row>
@@ -8185,17 +8261,17 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="70.6640625" style="8" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="8" bestFit="1" customWidth="1"/>
@@ -8258,24 +8334,26 @@
       <c r="A4" s="63" t="s">
         <v>474</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="88">
+      <c r="B4" s="66"/>
+      <c r="C4" s="85">
         <v>10</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="60" t="s">
+        <v>477</v>
+      </c>
       <c r="E4" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F4" s="65" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="71" customFormat="1" ht="17">
+    <row r="5" spans="1:6" s="69" customFormat="1" ht="17">
       <c r="A5" s="63" t="s">
         <v>374</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="69">
+      <c r="B5" s="66"/>
+      <c r="C5" s="67">
         <v>0</v>
       </c>
       <c r="D5" s="60" t="s">
@@ -8284,7 +8362,7 @@
       <c r="E5" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="65" t="s">
         <v>345</v>
       </c>
     </row>
@@ -8354,7 +8432,7 @@
       <c r="E9" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="65" t="s">
         <v>437</v>
       </c>
     </row>
@@ -8372,7 +8450,7 @@
       <c r="E10" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="65" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8390,7 +8468,7 @@
       <c r="E11" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="65" t="s">
         <v>346</v>
       </c>
     </row>
@@ -8408,7 +8486,7 @@
       <c r="E12" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="65" t="s">
         <v>347</v>
       </c>
     </row>
@@ -8426,7 +8504,7 @@
       <c r="E13" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="65" t="s">
         <v>348</v>
       </c>
     </row>
@@ -8444,7 +8522,7 @@
       <c r="E14" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="65" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8462,7 +8540,7 @@
       <c r="E15" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="65" t="s">
         <v>350</v>
       </c>
     </row>
@@ -8480,7 +8558,7 @@
       <c r="E16" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="66" t="s">
+      <c r="F16" s="65" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8498,7 +8576,7 @@
       <c r="E17" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="65" t="s">
         <v>352</v>
       </c>
     </row>
@@ -8516,7 +8594,7 @@
       <c r="E18" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="65" t="s">
         <v>353</v>
       </c>
     </row>
@@ -8534,7 +8612,7 @@
       <c r="E19" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="66" t="s">
+      <c r="F19" s="65" t="s">
         <v>354</v>
       </c>
     </row>
@@ -8552,58 +8630,72 @@
       <c r="E20" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="66" t="s">
+      <c r="F20" s="65" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="68" t="s">
         <v>341</v>
       </c>
       <c r="B21" s="64"/>
-      <c r="C21" s="65">
+      <c r="C21" s="92">
         <v>1</v>
       </c>
       <c r="D21" s="64"/>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17">
+      <c r="A22" s="68" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="62">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="64"/>
+      <c r="E22" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="66" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17">
-      <c r="A22" s="70" t="s">
-        <v>303</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="67">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="66" t="s">
+      <c r="F22" s="65" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="68" t="s">
         <v>304</v>
       </c>
       <c r="B23" s="64"/>
-      <c r="C23" s="67">
+      <c r="C23" s="93">
         <v>5</v>
       </c>
       <c r="D23" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="66" t="s">
+      <c r="F23" s="65" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C24" s="92">
+        <v>5000</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="65" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -8803,10 +8895,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="71" t="s">
         <v>392</v>
       </c>
-      <c r="B2" s="91">
+      <c r="B2" s="88">
         <v>50</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -8820,10 +8912,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="71" t="s">
         <v>393</v>
       </c>
-      <c r="B3" s="91">
+      <c r="B3" s="88">
         <v>3.5</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -8837,10 +8929,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="17">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="71" t="s">
         <v>394</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="88">
         <v>4.5</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -8854,10 +8946,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="71" t="s">
         <v>395</v>
       </c>
-      <c r="B5" s="91">
+      <c r="B5" s="88">
         <v>1</v>
       </c>
       <c r="C5" s="14"/>
@@ -8869,10 +8961,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="71" t="s">
         <v>396</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="88">
         <v>0</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -8886,10 +8978,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="71" t="s">
         <v>397</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="88">
         <v>150</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -8903,10 +8995,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="71" t="s">
         <v>398</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="88">
         <v>15</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -8920,10 +9012,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="71" t="s">
         <v>399</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="88">
         <v>25</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -8937,10 +9029,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="71" t="s">
         <v>400</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="88">
         <v>40</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -8954,10 +9046,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="17">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="71" t="s">
         <v>305</v>
       </c>
-      <c r="B11" s="92">
+      <c r="B11" s="89">
         <v>50</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -8971,10 +9063,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="34">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="B12" s="93">
+      <c r="B12" s="90">
         <v>20</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -8988,10 +9080,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="34">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="71" t="s">
         <v>379</v>
       </c>
-      <c r="B13" s="93">
+      <c r="B13" s="90">
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -9005,10 +9097,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="34">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="71" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="93">
+      <c r="B14" s="90">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -9022,10 +9114,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="34">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="71" t="s">
         <v>381</v>
       </c>
-      <c r="B15" s="93">
+      <c r="B15" s="90">
         <v>20</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -9039,10 +9131,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="34">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="71" t="s">
         <v>382</v>
       </c>
-      <c r="B16" s="93">
+      <c r="B16" s="90">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -9056,10 +9148,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="34">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="B17" s="93">
+      <c r="B17" s="90">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -9073,10 +9165,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="71" t="s">
         <v>384</v>
       </c>
-      <c r="B18" s="93">
+      <c r="B18" s="90">
         <v>20</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -9090,10 +9182,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="71" t="s">
         <v>385</v>
       </c>
-      <c r="B19" s="93">
+      <c r="B19" s="90">
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -9106,105 +9198,105 @@
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="72" customFormat="1" ht="34">
-      <c r="A20" s="73" t="s">
+    <row r="20" spans="1:5" s="70" customFormat="1" ht="34">
+      <c r="A20" s="71" t="s">
         <v>386</v>
       </c>
-      <c r="B20" s="94">
-        <v>0</v>
-      </c>
-      <c r="C20" s="72" t="s">
+      <c r="B20" s="91">
+        <v>0</v>
+      </c>
+      <c r="C20" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="74" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="72" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="74" t="s">
+    <row r="21" spans="1:5" s="70" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="72" t="s">
         <v>387</v>
       </c>
-      <c r="B21" s="94">
-        <v>0</v>
-      </c>
-      <c r="C21" s="72" t="s">
+      <c r="B21" s="91">
+        <v>0</v>
+      </c>
+      <c r="C21" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="76" t="s">
+      <c r="D21" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="76" t="s">
+      <c r="E21" s="74" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="72" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:5" s="70" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A22" s="71" t="s">
         <v>388</v>
       </c>
-      <c r="B22" s="94">
+      <c r="B22" s="91">
         <v>20</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="76" t="s">
+      <c r="D22" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="74" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="72" customFormat="1" ht="17" customHeight="1">
-      <c r="A23" s="73" t="s">
+    <row r="23" spans="1:5" s="70" customFormat="1" ht="17" customHeight="1">
+      <c r="A23" s="71" t="s">
         <v>389</v>
       </c>
-      <c r="B23" s="94">
-        <v>0</v>
-      </c>
-      <c r="C23" s="72" t="s">
+      <c r="B23" s="91">
+        <v>0</v>
+      </c>
+      <c r="C23" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="76" t="s">
+      <c r="D23" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E23" s="74" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="72" customFormat="1" ht="34">
-      <c r="A24" s="73" t="s">
+    <row r="24" spans="1:5" s="70" customFormat="1" ht="34">
+      <c r="A24" s="71" t="s">
         <v>390</v>
       </c>
-      <c r="B24" s="94">
-        <v>0</v>
-      </c>
-      <c r="C24" s="72" t="s">
+      <c r="B24" s="91">
+        <v>0</v>
+      </c>
+      <c r="C24" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="76" t="s">
+      <c r="E24" s="74" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="72" customFormat="1" ht="17">
-      <c r="A25" s="73" t="s">
+    <row r="25" spans="1:5" s="70" customFormat="1" ht="17">
+      <c r="A25" s="71" t="s">
         <v>391</v>
       </c>
-      <c r="B25" s="94">
+      <c r="B25" s="91">
         <v>100</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="76" t="s">
+      <c r="D25" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="76" t="s">
+      <c r="E25" s="74" t="s">
         <v>369</v>
       </c>
     </row>
@@ -10137,7 +10229,7 @@
       <c r="B30" s="33" t="s">
         <v>423</v>
       </c>
-      <c r="C30" s="77">
+      <c r="C30" s="75">
         <v>100</v>
       </c>
       <c r="D30" s="30" t="s">

</xml_diff>

<commit_message>
start changes in boxes
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v17.xlsx
+++ b/Template_CoMoCOVID-19App_v17.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF0776F-07E2-5049-95A5-4AAB3995960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB4E26E-6E4C-0142-8009-6F88F1967BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="640" windowWidth="24880" windowHeight="20680" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="5660" yWindow="2400" windowWidth="32740" windowHeight="19200" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Epidemiology" sheetId="2" r:id="rId2"/>
     <sheet name="Severity-Mortality" sheetId="4" r:id="rId3"/>
     <sheet name="Population" sheetId="3" r:id="rId4"/>
     <sheet name="Parameters" sheetId="13" r:id="rId5"/>
@@ -23,7 +23,7 @@
     <sheet name="Hospitalisation Param" sheetId="9" r:id="rId8"/>
     <sheet name="Interventions Param" sheetId="11" r:id="rId9"/>
     <sheet name="Interventions" sheetId="14" r:id="rId10"/>
-    <sheet name="HIDDEN" sheetId="12" r:id="rId11"/>
+    <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$31</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="484">
   <si>
     <t>5-10 y.o.</t>
   </si>
@@ -2627,9 +2627,6 @@
     <t>1-5; 21</t>
   </si>
   <si>
-    <t>1-3; 8; 19-21</t>
-  </si>
-  <si>
     <t>Age Groups</t>
   </si>
   <si>
@@ -2980,6 +2977,12 @@
     </r>
   </si>
   <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>Seroprevalence (e.g. 12.3 for 12.3%)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -2991,16 +2994,60 @@
     <r>
       <rPr>
         <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Average sample size for seroprevalence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Renamed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Sample Size</t>
-    </r>
-  </si>
-  <si>
-    <t>(a)</t>
+      <t>Cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epidemiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Added a column for Seroprevalence survey data.</t>
+    </r>
+  </si>
+  <si>
+    <t>v17.b</t>
   </si>
 </sst>
 </file>
@@ -3010,9 +3057,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3114,6 +3161,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="10">
@@ -3265,7 +3321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3475,29 +3531,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3542,6 +3589,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3556,14 +3613,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="E1:F15" xr:uid="{2E89BE7F-E667-6946-928D-DC5AB4119A65}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3866,7 +3923,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3882,7 +3939,7 @@
         <v>438</v>
       </c>
       <c r="B1" s="95" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21">
@@ -3912,7 +3969,7 @@
     </row>
     <row r="8" spans="1:6" ht="89" customHeight="1">
       <c r="A8" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3920,93 +3977,93 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="94" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="94" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="94" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="94" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="94" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="94" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="94" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="94" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="94" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="94" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F24" s="40"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="94" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F25" s="40"/>
     </row>
     <row r="26" spans="1:6" s="39" customFormat="1">
       <c r="A26" s="94" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B26"/>
       <c r="D26"/>
@@ -4014,171 +4071,176 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="94" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F27" s="40"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="94" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="94" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F29" s="40"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="94" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="94" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F31" s="40"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="94" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F32" s="40"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="94" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="94" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F34" s="40"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="94" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F35" s="40"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="78" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34">
       <c r="A38" s="86" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="34">
       <c r="A39" s="87" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34">
       <c r="A40" s="87" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17">
       <c r="A41" s="87" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="78"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="81" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17">
+      <c r="A42" s="87" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="78"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="81" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="34">
-      <c r="A45" s="38" t="s">
+    <row r="46" spans="1:6" ht="34">
+      <c r="A46" s="38" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="17">
-      <c r="A46" s="38" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17">
       <c r="A47" s="38" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17">
       <c r="A48" s="38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="17">
+      <c r="A49" s="38" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="34">
-      <c r="A49" s="38" t="s">
+    <row r="50" spans="1:1" ht="34">
+      <c r="A50" s="38" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="76" t="s">
+    <row r="52" spans="1:1">
+      <c r="A52" s="76" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="40" t="s">
+    <row r="53" spans="1:1">
+      <c r="A53" s="40" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="77" t="s">
+    <row r="55" spans="1:1">
+      <c r="A55" s="77" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="34">
-      <c r="A56" s="38" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="34">
       <c r="A57" s="38" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="34">
+      <c r="A58" s="38" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="68">
-      <c r="A58" s="38" t="s">
+    <row r="59" spans="1:1" ht="68">
+      <c r="A59" s="38" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="38"/>
-    </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="77" t="s">
+      <c r="A60" s="38"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="77" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4195,7 +4257,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -4227,7 +4289,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>270</v>
@@ -4493,7 +4555,7 @@
         <v>thousand tests</v>
       </c>
       <c r="F13" s="84" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>278</v>
@@ -4517,7 +4579,7 @@
         <v>%</v>
       </c>
       <c r="F14" s="84" t="s">
-        <v>441</v>
+        <v>479</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>278</v>
@@ -5579,7 +5641,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F100">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>NOT(OR($A2 = "Vaccination", $A2 = "School Closures",  $A2 = "Mass Testing"))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6510,17 +6572,21 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="3" width="11" style="1"/>
-    <col min="4" max="16384" width="11" style="8"/>
+    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="68">
+    <row r="1" spans="1:4" ht="68">
       <c r="A1" s="9" t="s">
         <v>280</v>
       </c>
@@ -6530,8 +6596,11 @@
       <c r="C1" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="7">
         <v>43830</v>
       </c>
@@ -6542,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="7">
         <v>43831</v>
       </c>
@@ -6553,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="7">
         <v>43832</v>
       </c>
@@ -6564,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="7">
         <v>43833</v>
       </c>
@@ -6575,7 +6644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="7">
         <v>43834</v>
       </c>
@@ -6586,7 +6655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="7">
         <v>43835</v>
       </c>
@@ -6597,7 +6666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="7">
         <v>43836</v>
       </c>
@@ -6608,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="7">
         <v>43837</v>
       </c>
@@ -6619,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="7">
         <v>43838</v>
       </c>
@@ -6630,7 +6699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="7">
         <v>43839</v>
       </c>
@@ -6641,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="7">
         <v>43840</v>
       </c>
@@ -6652,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="7">
         <v>43841</v>
       </c>
@@ -6663,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="7">
         <v>43842</v>
       </c>
@@ -6674,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="7">
         <v>43843</v>
       </c>
@@ -6685,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="7">
         <v>43844</v>
       </c>
@@ -7651,7 +7720,9 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -7674,7 +7745,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B2" s="78">
         <v>1.6000000000000001E-3</v>
@@ -7922,7 +7993,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7951,7 +8022,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B2" s="79">
         <v>3924000</v>
@@ -8263,8 +8334,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -8332,14 +8403,14 @@
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" s="63" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B4" s="66"/>
       <c r="C4" s="85">
         <v>10</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E4" s="59" t="s">
         <v>23</v>
@@ -8438,7 +8509,7 @@
     </row>
     <row r="10" spans="1:6" ht="17">
       <c r="A10" s="63" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B10" s="60"/>
       <c r="C10" s="62">
@@ -8685,8 +8756,8 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="8" t="s">
-        <v>480</v>
+      <c r="A24" s="96" t="s">
+        <v>481</v>
       </c>
       <c r="C24" s="92">
         <v>5000</v>
@@ -8695,7 +8766,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="65" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -8862,7 +8933,7 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data incl. severity/mortality
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v17.xlsx
+++ b/Template_CoMoCOVID-19App_v17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB4E26E-6E4C-0142-8009-6F88F1967BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B162C87-E621-384C-A188-6A2C4C7C1A36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="2400" windowWidth="32740" windowHeight="19200" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="5880" yWindow="500" windowWidth="22280" windowHeight="17500" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3047,7 +3047,7 @@
     </r>
   </si>
   <si>
-    <t>v17.b</t>
+    <t>v17.c</t>
   </si>
 </sst>
 </file>
@@ -7721,14 +7721,14 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -7748,10 +7748,10 @@
         <v>475</v>
       </c>
       <c r="B2" s="78">
-        <v>1.6000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="78">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7759,10 +7759,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="78">
-        <v>1.6000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="78">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -7770,10 +7770,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="78">
-        <v>7.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="78">
-        <v>0.04</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -7781,10 +7781,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="78">
-        <v>7.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="78">
-        <v>0.04</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -7792,7 +7792,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="78">
-        <v>3.1E-2</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="78">
         <v>1.1000000000000001</v>
@@ -7803,7 +7803,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="78">
-        <v>3.1E-2</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="78">
         <v>1.1000000000000001</v>
@@ -7814,10 +7814,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="78">
-        <v>0.26</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="C8" s="78">
-        <v>3.43</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -7825,10 +7825,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="78">
-        <v>0.26</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="C9" s="78">
-        <v>3.43</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -7836,10 +7836,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="78">
-        <v>0.48</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="C10" s="78">
-        <v>4.25</v>
+        <v>3.3000000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -7847,10 +7847,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="78">
-        <v>0.48</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="C11" s="78">
-        <v>4.25</v>
+        <v>3.3000000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -7858,10 +7858,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="78">
-        <v>0.6</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="C12" s="78">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -7869,10 +7869,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="78">
-        <v>0.6</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="C13" s="78">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -7880,10 +7880,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="78">
-        <v>1.9</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="C14" s="78">
-        <v>11.8</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -7891,10 +7891,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="78">
-        <v>1.9</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="C15" s="78">
-        <v>11.8</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -7902,10 +7902,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="78">
-        <v>4.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C16" s="78">
-        <v>16.600000000000001</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -7913,10 +7913,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="78">
-        <v>4.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C17" s="78">
-        <v>16.600000000000001</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -7924,10 +7924,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="78">
-        <v>7.8</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="C18" s="78">
-        <v>18.399999999999999</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -7935,10 +7935,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="78">
-        <v>7.8</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="C19" s="78">
-        <v>18.399999999999999</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -7946,10 +7946,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="78">
-        <v>7.8</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="C20" s="78">
-        <v>18.399999999999999</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -7957,10 +7957,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="78">
-        <v>7.8</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="C21" s="78">
-        <v>18.399999999999999</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -7968,10 +7968,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="78">
-        <v>7.8</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="C22" s="78">
-        <v>18.399999999999999</v>
+        <v>31.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avg sample size for seroprevalence default to 100
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v17.xlsx
+++ b/Template_CoMoCOVID-19App_v17.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B162C87-E621-384C-A188-6A2C4C7C1A36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EFA703-5080-CB49-BA76-16F1144198C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="500" windowWidth="22280" windowHeight="17500" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="5920" yWindow="500" windowWidth="20360" windowHeight="17500" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3047,7 +3047,7 @@
     </r>
   </si>
   <si>
-    <t>v17.c</t>
+    <t>v17.d</t>
   </si>
 </sst>
 </file>
@@ -3055,9 +3055,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -3319,7 +3319,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3389,7 +3389,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3495,7 +3495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3528,10 +3528,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3925,7 +3925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6575,8 +6575,8 @@
   <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7293,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:4">
       <c r="A65" s="7">
         <v>43893</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:4">
       <c r="A66" s="7">
         <v>43894</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:4">
       <c r="A67" s="7">
         <v>43895</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:4">
       <c r="A68" s="7">
         <v>43896</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:4">
       <c r="A69" s="7">
         <v>43897</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:4">
       <c r="A70" s="7">
         <v>43898</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:4">
       <c r="A71" s="7">
         <v>43899</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:4">
       <c r="A72" s="7">
         <v>43900</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:4">
       <c r="A73" s="7">
         <v>43901</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:4">
       <c r="A74" s="7">
         <v>43902</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:4">
       <c r="A75" s="7">
         <v>43903</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:4">
       <c r="A76" s="7">
         <v>43904</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:4">
       <c r="A77" s="7">
         <v>43905</v>
       </c>
@@ -7435,8 +7435,11 @@
       <c r="C77" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="7">
         <v>43906</v>
       </c>
@@ -7447,7 +7450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:4">
       <c r="A79" s="7">
         <v>43907</v>
       </c>
@@ -7458,7 +7461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:4">
       <c r="A80" s="7">
         <v>43908</v>
       </c>
@@ -7469,7 +7472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:4">
       <c r="A81" s="7">
         <v>43909</v>
       </c>
@@ -7480,7 +7483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:4">
       <c r="A82" s="7">
         <v>43910</v>
       </c>
@@ -7490,8 +7493,11 @@
       <c r="C82" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="7">
         <v>43911</v>
       </c>
@@ -7502,7 +7508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:4">
       <c r="A84" s="7">
         <v>43912</v>
       </c>
@@ -7513,7 +7519,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:4">
       <c r="A85" s="7">
         <v>43913</v>
       </c>
@@ -7524,7 +7530,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:4">
       <c r="A86" s="7">
         <v>43914</v>
       </c>
@@ -7535,7 +7541,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:4">
       <c r="A87" s="7">
         <v>43915</v>
       </c>
@@ -7545,8 +7551,11 @@
       <c r="C87" s="1">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="7">
         <v>43916</v>
       </c>
@@ -7557,7 +7566,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:4">
       <c r="A89" s="7">
         <v>43917</v>
       </c>
@@ -7568,7 +7577,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:4">
       <c r="A90" s="7">
         <v>43918</v>
       </c>
@@ -7579,7 +7588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:4">
       <c r="A91" s="7">
         <v>43919</v>
       </c>
@@ -7590,7 +7599,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:4">
       <c r="A92" s="7">
         <v>43920</v>
       </c>
@@ -7600,8 +7609,11 @@
       <c r="C92" s="1">
         <v>209</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92" s="1">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="7">
         <v>43921</v>
       </c>
@@ -7612,7 +7624,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:4">
       <c r="A94" s="7">
         <v>43922</v>
       </c>
@@ -7623,7 +7635,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:4">
       <c r="A95" s="7">
         <v>43923</v>
       </c>
@@ -7634,7 +7646,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:4">
       <c r="A96" s="7">
         <v>43924</v>
       </c>
@@ -8334,7 +8346,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -8760,7 +8772,7 @@
         <v>481</v>
       </c>
       <c r="C24" s="92">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="E24" s="65" t="s">
         <v>23</v>
@@ -8933,7 +8945,7 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>